<commit_message>
Ajout des Etats Spirituels (que j'avais oublié)
</commit_message>
<xml_diff>
--- a/Etats.xlsx
+++ b/Etats.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC52CCC-DAA5-44DF-AAB5-33E7D1456F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="6_{6E36F479-7684-4CB8-A20A-2417758874EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDD9E4CF-A079-48B0-AE9A-943C1FF8DCB0}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="2895" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etats" sheetId="1" r:id="rId1"/>
-    <sheet name="Tilts" sheetId="2" r:id="rId2"/>
+    <sheet name="Etats Spirituels" sheetId="3" r:id="rId2"/>
+    <sheet name="Tilts" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Etats!$A$1:$F$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tilts!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Etats Spirituels'!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tilts!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="411">
   <si>
     <t>Nom</t>
   </si>
@@ -1140,6 +1140,151 @@
   </si>
   <si>
     <t xml:space="preserve">A character can be stunned by any attack that does at least as much damage as her Size in a single hit. Some weapons have a “stun” special ability. These double the weapon modifier only for the purposes of determining whether the attacker inflicts the Stunned Tilt. Attacks against the target’s head (see “Specified Targets,” p. 203) count the character’s Size as one lower for the purposes of this Tilt. The Storyteller might determine that additional effects cause this Tilt, like being caught in the blast area of an explosion (World of Darkness Rulebook, p. 178). </t>
+  </si>
+  <si>
+    <t>RESONANT</t>
+  </si>
+  <si>
+    <t>The subject of this Condition is within the sphere of influence of a spirit.</t>
+  </si>
+  <si>
+    <t>This Condition is common and naturally-occurring — if an object, phenomenon, person, or place matches the spirit’s purview in some way, it has this Condition. Anything matching the description of one of a spirit’s Influences counts as having this Condition tagged to the spirit. Summoning rites intended to entice a particular spirit to a location work by instilling the qualities that result in this Condition. Finally, a high-Rank spirit can use a Create Influence to cause the prerequisites for the Condition itself.</t>
+  </si>
+  <si>
+    <t>The Condition ends if the phenomenon creating it ends. A forest stops being Resonant for a tree spirit when humans fell all the trees, a grief spirit can’t Influence someone who has healed and let go of his pain, and a fire spirit must move on when the fire is extinguished. Banishing rites may temporarily suppress the Condition.</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>The place, object, animal, or person covered by a Resonant Condition is now conditioned to accept the resonant spirit. That spirit can now attempt to Fetter itself to the subject of the Condition, or, if the Condition is on a location, Materialize.</t>
+  </si>
+  <si>
+    <t>Prérequis</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>The Resonant Condition for the same phenomenon to which this Condition is tagged.</t>
+  </si>
+  <si>
+    <t>This Condition is usually the result of fine-tuning the Resonant Condition as part of an extended action, involving the subject and spirit acting in concert for a number of scenes equal to Rank or a living subject’s Resolve, whichever is higher. Using a Strengthen Influence allows a spirit to temporarily upgrade Resonant to Open as an instant action. Last, both Lunacy and some Wolf-Blooded Tells can cause Open spontaneously, offering the subject up to a spirit without any effort on its part.</t>
+  </si>
+  <si>
+    <t>The Condition ends if the prerequisite Condition is removed. Exorcism rites work by removing this Condition, reverting it to the prerequisite</t>
+  </si>
+  <si>
+    <t>CONTROLLED</t>
+  </si>
+  <si>
+    <t>The object, creature, or person covered by an Open Condition has now been so conditioned that the spirit may attempt to Claim it, permanently merging with it.</t>
+  </si>
+  <si>
+    <t>The intended subject of this Condition must have the Open Condition, tagged to the spirit attempting to cause it.</t>
+  </si>
+  <si>
+    <t>This Condition is the result of repeated use of the Possess Manifestation Effect by the causing spirit. It must have succeeded in possessing the subject on a number of separate occasions equal to the Willpower of spirit or subject (whichever is higher). If any Possessed Condition is removed before its duration ends, the spirit loses any progress on building to the required number of possessions.</t>
+  </si>
+  <si>
+    <t>Successfully ending the Controlled Condition, or a Claimed Condition resulting from it, against the spirit’s will removes this Condition and reverts the subject to Open.</t>
+  </si>
+  <si>
+    <t>REACHING</t>
+  </si>
+  <si>
+    <t>The spirit has opened a conduit through the Gauntlet, allowing it to use Influences and Numina to affect the other side. Numina with [R] after their name can be used with this Condition. Characters capable of perceiving spirits in Twilight can sense the conduit’s presence with a successful Wits + Composure roll.</t>
+  </si>
+  <si>
+    <t>This Condition is the result of the Reaching Manifestation Effect and lasts for one Scene.</t>
+  </si>
+  <si>
+    <t>At the end of the scene, theCondition fades.</t>
+  </si>
+  <si>
+    <t>SHADOW GATE</t>
+  </si>
+  <si>
+    <t>The location has a hole punched through the Gauntlet. Spirits, packs — and even incautious humans — can cross through it without the use of any powers. The Shadow Gate is visible even to material beings, as the Shadow world and material worlds mix.</t>
+  </si>
+  <si>
+    <t>This Condition can be created by using the Shadow Gateway Manifestation Effect on an Open Condition.</t>
+  </si>
+  <si>
+    <t>At the end of the scene, the
+Condition fades.</t>
+  </si>
+  <si>
+    <t>MATERIALIZED</t>
+  </si>
+  <si>
+    <t>The spirit has shifted from ephemeral to material substance, Manifesting in physical form. All the rules for ephemeral spirit’s traits still apply except for the effects of being in Twilight. This Condition protects the spirit from Essence bleed for its duration.</t>
+  </si>
+  <si>
+    <t>This Condition is created by a spirit using the Materialize Manifestation Effect on an Open Condition. If the Open Condition used is on an object or person, the spirit must materialize within its Rank in yards.</t>
+  </si>
+  <si>
+    <t>Materialization lasts for one hour per success on the activating roll. When the duration ends, the spirit fades back into Twilight. Physical contact with a Bane or removal of a prerequisite Condition causes the Condition to end early.</t>
+  </si>
+  <si>
+    <t>FETTERED</t>
+  </si>
+  <si>
+    <t>The spirit has secured itself to an object or creature. As long as it remains Fettered, the spirit is safe from Essence bleed. The spirit remains in Twilight and must stay within five yards of the Fetter. Most spirits Fettering themselves literally hide inside their Fetters if they are small enough.
+The spirit pays one less Essence for using Influences on the Fetter, but may not use them or Numina on another target as long as the Fetter lasts.</t>
+  </si>
+  <si>
+    <t>This Condition is created by a spirit using the Fetter Manifestation Effect.</t>
+  </si>
+  <si>
+    <t>Fetters are permanent unless the prerequisite Conditions are ended, or if the subject of the Fetter is destroyed or killed (if a living being). The spirit can voluntarily end the Condition by using the Unfetter Manifestation Effect.</t>
+  </si>
+  <si>
+    <t>URGED</t>
+  </si>
+  <si>
+    <t>This animal or human host has been used as a Fetter by a spirit. The spirit may read the subject’s thoughts with a successful Power + Finesse roll, contested by Resolve + Primal Urge. Success reveals surface thoughts. The spirit may urge the host to take a specified action with a successful Power + Finesse roll contested by Resolve + Composure. If the spirit wins, it creates the urge. Following the urge rewards the host with a Beat.</t>
+  </si>
+  <si>
+    <t>The Urged Condition ends whenever the linked Fetter ends.</t>
+  </si>
+  <si>
+    <t>POSSESSED</t>
+  </si>
+  <si>
+    <t>This object, corpse, or living being is temporarily controlled by a spirit. Living hosts are put into a coma-like state while being possessed — they experience the possession as missing time, except for flashbacks that might come out in dreams or times of stress such as losing Integrity. The spirit may not use Numina or Influences while controlling the host,but is safe from Essence bleed as long as the possession lasts.
+The spirit may pay one Essence per turn to heal one lethal or bashing wound or a point of structure lost to damage. A corpse that died through damage begins Possession incapacitated.
+Spirits possessing inanimate objects or corpses have a great deal of control over their host. A spirit controlling an object can’t make it do anything it couldn’t do while being operated, but it can turn switches on and off, operate machinery, use keyboards, and turn dials. Use the spirit’s Finesse if dice rolls are necessary.
+Corpses and other articulated hosts capable of movement, such as shop mannequins or industrial robots, use their own Physical Attributes but the spirit’s Attributes in Social or Mental rolls. By spending a point of Essence, the spirit can use its own Attributes instead of the host’s for Physical tasks for a turn, but doing so causes one point of lethal damage or structure loss to the host. 
+Living hosts require more time for the spirit to gain full control and always use the host’s own Attributes. The spirit may read the host’s mind with a Finesse Roll at a –4 penalty, use the host’s Physical Skills at a –3 penalty, and the host’s Social and Mental Skills at –4. Reduce these penalties by one die per day that the spirit has been Fettered to the host. Most possessing spirits Fetter themselves to their intended hosts and use the Possess Manifestation Effect to take full control only in emergencies.
+To possess a host, the spirit must remain in Twilight, superimposed over the host. This means that if the host touches the spirit’s bane or is injured by a weapon made of the bane, the spirit will suffer wounds to its Corpus.</t>
+  </si>
+  <si>
+    <t>This Condition is created by a spirit using the Possess Manifestation Effect.</t>
+  </si>
+  <si>
+    <t>The object or victim must be under the Open Condition, tagged to the spirit.</t>
+  </si>
+  <si>
+    <t>The possession lasts for a single scene, unless the spirit abandons it early or the host is killed or destroyed. Abjurations, exorcisms and forced contact with banes and bans can all motivate a spirit to release a host.</t>
+  </si>
+  <si>
+    <t>CLAIMED</t>
+  </si>
+  <si>
+    <t>A Claimed object, corpse, creature, or person is permanently possessed and merges with the spirit involved. Unlike victims of Possess, a living Claimed isn’t put into a fugue state, but remains mentally active while his soul and the Claiming spirit merge together over the course of several days. During the period of fusion, the subject is under all the effects of the Urged Condition, described above. Once per day, starting with the moment the Claimed Condition is created, add one dot of the spirit’s Attributes to the host’s, permanently raising them. Power may be assigned to Strength, Intelligence, or Presence, Finesse to Wits, Dexterity, or Manipulation, and Resistance to Stamina, Composure, or Resolve. The host’s physical form begins to mutate, taking on an appearance influenced by the original host and the spirit.
+Claimed corpses add dots to Attributes as above, but start with all Mental and Social Attributes at 0. Inanimate objects begin with Dexterity 0, but use Structure and Durability instead of Strength and also start the claiming process with all Mental and Social Attributes at 0. Corpses and inanimate hosts don’t spend the claiming period under the Urged Condition, having no minds of their own to warp.
+Claimed may use the spirit’s Influences, but not Numinaor Manifestation Effects. They may develop unique Dread Powers (p. 210). From the moment the Claimed Condition starts, the spirit is safe from Essence bleed. The hybrid being that results has the spirit’s Essence trait, ban, and bane, but is a material being. Claimed that were once spirits may cross the Gauntlet at a Locus with a successful Intelligence + Presence roll. Claimed that were inanimate objects are fully animate, fusions of spiritual power, metal, and plastic.</t>
+  </si>
+  <si>
+    <t>Claim is permanent in living hosts unless the spirit decides to detach itself, rolling its original Power + Finesse penalized by its own Rank and contested by the Claimed host’s Resolve + Composure — including any dots gained from being Claimed. If the spirit succeeds, it separates from the host. Former hosts are physically and mentally scarred — their physical appearance changes back at the same rate it mutated and the extra Attribute dots fade at a rate of two per day. The Essence trait and any Dread Powers the Claimed developed immediately vanish.
+In nonliving hosts, Claim is only temporary — once the Claim has fully formed, the host loses one dot of a Physical Attribute (or equivalent for formerly inanimate objects) per three days. When any of these Attributes reaches 0, the host disintegrates and the spirit is released into Twilight.</t>
+  </si>
+  <si>
+    <t>This Condition is created by a spirit using the Claim Manifestation Effect.</t>
+  </si>
+  <si>
+    <t>The object or victim must be under the Controlled Condition, tagged to the spirit.</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1222,6 +1367,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,23 +1657,23 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
+      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="80" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>56</v>
       </c>
@@ -1542,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>58</v>
       </c>
@@ -1562,7 +1713,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
@@ -1582,7 +1733,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>57</v>
       </c>
@@ -1602,7 +1753,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
@@ -1622,7 +1773,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
@@ -1642,7 +1793,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -1662,7 +1813,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
@@ -1682,7 +1833,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>58</v>
       </c>
@@ -1702,7 +1853,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
@@ -1722,7 +1873,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>57</v>
       </c>
@@ -1742,7 +1893,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>58</v>
       </c>
@@ -1762,7 +1913,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -1782,7 +1933,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
@@ -1802,7 +1953,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
@@ -1822,7 +1973,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>57</v>
       </c>
@@ -1842,7 +1993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>58</v>
       </c>
@@ -1862,7 +2013,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -1882,7 +2033,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>57</v>
       </c>
@@ -1902,7 +2053,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
@@ -1922,7 +2073,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>57</v>
       </c>
@@ -1942,7 +2093,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>57</v>
       </c>
@@ -1962,7 +2113,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>58</v>
       </c>
@@ -1982,7 +2133,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>57</v>
       </c>
@@ -2002,7 +2153,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>57</v>
       </c>
@@ -2022,7 +2173,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>58</v>
       </c>
@@ -2042,7 +2193,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>57</v>
       </c>
@@ -2062,7 +2213,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
@@ -2082,7 +2233,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>57</v>
       </c>
@@ -2102,7 +2253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>58</v>
       </c>
@@ -2122,7 +2273,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>57</v>
       </c>
@@ -2142,7 +2293,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>57</v>
       </c>
@@ -2162,7 +2313,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>57</v>
       </c>
@@ -2182,7 +2333,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>58</v>
       </c>
@@ -2202,7 +2353,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
@@ -2222,7 +2373,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>57</v>
       </c>
@@ -2242,7 +2393,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="171" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>57</v>
       </c>
@@ -2262,7 +2413,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>57</v>
       </c>
@@ -2282,7 +2433,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>58</v>
       </c>
@@ -2302,7 +2453,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>57</v>
       </c>
@@ -2322,7 +2473,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>58</v>
       </c>
@@ -2342,7 +2493,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>57</v>
       </c>
@@ -2362,7 +2513,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>58</v>
       </c>
@@ -2382,7 +2533,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>58</v>
       </c>
@@ -2402,7 +2553,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>57</v>
       </c>
@@ -2422,7 +2573,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>57</v>
       </c>
@@ -2442,7 +2593,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>57</v>
       </c>
@@ -2462,7 +2613,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>57</v>
       </c>
@@ -2482,7 +2633,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>57</v>
       </c>
@@ -2502,7 +2653,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>57</v>
       </c>
@@ -2522,7 +2673,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>57</v>
       </c>
@@ -2542,7 +2693,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>58</v>
       </c>
@@ -2562,7 +2713,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>57</v>
       </c>
@@ -2582,7 +2733,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>57</v>
       </c>
@@ -2602,7 +2753,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>58</v>
       </c>
@@ -2622,7 +2773,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>57</v>
       </c>
@@ -2642,7 +2793,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>58</v>
       </c>
@@ -2662,7 +2813,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>57</v>
       </c>
@@ -2682,7 +2833,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>57</v>
       </c>
@@ -2702,7 +2853,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>57</v>
       </c>
@@ -2722,7 +2873,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>58</v>
       </c>
@@ -2742,7 +2893,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>57</v>
       </c>
@@ -2762,7 +2913,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>57</v>
       </c>
@@ -2782,7 +2933,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>57</v>
       </c>
@@ -2802,7 +2953,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>57</v>
       </c>
@@ -2830,27 +2981,240 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14D36AE-BE73-4E04-92BC-36477B6C6F8A}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="72.85546875" customWidth="1"/>
+    <col min="5" max="5" width="50.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="360" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>408</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E2" xr:uid="{517F8BE9-D1B5-48B3-A4BB-2CB3126EB213}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55C0BB8-057D-47B4-9ABC-18D1A275BB50}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="89.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>56</v>
       </c>
@@ -2870,7 +3234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>57</v>
       </c>
@@ -2890,7 +3254,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
@@ -2910,7 +3274,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
@@ -2930,7 +3294,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>57</v>
       </c>
@@ -2950,7 +3314,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>58</v>
       </c>
@@ -2970,7 +3334,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>58</v>
       </c>
@@ -2990,7 +3354,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
@@ -3010,7 +3374,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>58</v>
       </c>
@@ -3030,7 +3394,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>57</v>
       </c>
@@ -3050,7 +3414,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>58</v>
       </c>
@@ -3070,7 +3434,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>58</v>
       </c>
@@ -3090,7 +3454,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>58</v>
       </c>
@@ -3110,7 +3474,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>58</v>
       </c>
@@ -3130,7 +3494,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>58</v>
       </c>
@@ -3150,7 +3514,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>57</v>
       </c>
@@ -3170,7 +3534,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>58</v>
       </c>
@@ -3190,7 +3554,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
@@ -3210,7 +3574,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
@@ -3230,7 +3594,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="285" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>58</v>
       </c>
@@ -3250,7 +3614,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>58</v>
       </c>
@@ -3270,7 +3634,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>57</v>
       </c>
@@ -3290,7 +3654,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>58</v>
       </c>
@@ -3310,7 +3674,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>57</v>
       </c>
@@ -3330,7 +3694,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>58</v>
       </c>
@@ -3350,7 +3714,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>57</v>
       </c>
@@ -3370,7 +3734,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>58</v>
       </c>
@@ -3390,7 +3754,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
@@ -3410,7 +3774,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>57</v>
       </c>
@@ -3430,7 +3794,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>58</v>
       </c>

</xml_diff>